<commit_message>
se arregló url en el DataSource - Pago.xlsx para que ande en BC
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Pago.xlsx
+++ b/Sura/DataSource - Pago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992634F7-ECBF-40A8-B01A-52D99FC7C502}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D141FBD6-CFD7-420E-9647-CCED558DE7C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,9 +60,6 @@
     <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
   </si>
   <si>
-    <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/pc/PolicyCenter.do</t>
-  </si>
-  <si>
     <t>gw</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/bc/BillingCenter.do</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A53"/>
+      <selection activeCell="C2" sqref="C2:C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +577,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -612,22 +612,22 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>1312</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="G2">
-        <v>1312</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="I2" t="s">
         <v>7</v>
@@ -641,22 +641,22 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3">
         <v>1312</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
@@ -670,22 +670,22 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4">
         <v>1312</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I4" t="s">
         <v>7</v>
@@ -699,22 +699,22 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5">
         <v>1312</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
         <v>7</v>
@@ -728,22 +728,22 @@
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6">
         <v>1312</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" t="s">
         <v>7</v>
@@ -757,22 +757,22 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7">
         <v>1312</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I7" t="s">
         <v>7</v>
@@ -786,22 +786,22 @@
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8">
         <v>1312</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s">
         <v>7</v>
@@ -815,22 +815,22 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9">
         <v>1312</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I9" t="s">
         <v>7</v>
@@ -844,22 +844,22 @@
         <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10">
         <v>1312</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" t="s">
         <v>7</v>
@@ -873,22 +873,22 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11">
         <v>1312</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I11" t="s">
         <v>7</v>
@@ -902,22 +902,22 @@
         <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G12">
         <v>1312</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I12" t="s">
         <v>7</v>
@@ -931,22 +931,22 @@
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G13">
         <v>1312</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I13" t="s">
         <v>7</v>
@@ -960,22 +960,22 @@
         <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G14">
         <v>1312</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I14" t="s">
         <v>7</v>
@@ -989,22 +989,22 @@
         <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G15">
         <v>1312</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I15" t="s">
         <v>7</v>
@@ -1018,22 +1018,22 @@
         <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G16">
         <v>1312</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I16" t="s">
         <v>7</v>
@@ -1047,22 +1047,22 @@
         <v>10</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G17">
         <v>1312</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I17" t="s">
         <v>7</v>
@@ -1076,22 +1076,22 @@
         <v>10</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G18">
         <v>1312</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I18" t="s">
         <v>7</v>
@@ -1105,22 +1105,22 @@
         <v>10</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G19">
         <v>1312</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I19" t="s">
         <v>7</v>
@@ -1134,22 +1134,22 @@
         <v>10</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G20">
         <v>1312</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I20" t="s">
         <v>7</v>
@@ -1163,22 +1163,22 @@
         <v>10</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G21">
         <v>1312</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I21" t="s">
         <v>7</v>
@@ -1192,22 +1192,22 @@
         <v>10</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G22">
         <v>1312</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I22" t="s">
         <v>7</v>
@@ -1221,22 +1221,22 @@
         <v>10</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G23">
         <v>1312</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I23" t="s">
         <v>7</v>
@@ -1250,22 +1250,22 @@
         <v>10</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G24">
         <v>1312</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I24" t="s">
         <v>7</v>
@@ -1279,22 +1279,22 @@
         <v>10</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G25">
         <v>1312</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I25" t="s">
         <v>7</v>
@@ -1308,22 +1308,22 @@
         <v>10</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G26">
         <v>1312</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I26" t="s">
         <v>7</v>
@@ -1337,22 +1337,22 @@
         <v>10</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G27">
         <v>1312</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I27" t="s">
         <v>7</v>
@@ -1366,22 +1366,22 @@
         <v>10</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G28">
         <v>1312</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I28" t="s">
         <v>7</v>
@@ -1395,22 +1395,22 @@
         <v>10</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G29">
         <v>1312</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I29" t="s">
         <v>7</v>
@@ -1424,22 +1424,22 @@
         <v>10</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D30" t="s">
         <v>6</v>
       </c>
       <c r="E30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G30">
         <v>1312</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I30" t="s">
         <v>7</v>
@@ -1453,22 +1453,22 @@
         <v>10</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G31">
         <v>1312</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I31" t="s">
         <v>7</v>
@@ -1482,22 +1482,22 @@
         <v>10</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D32" t="s">
         <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G32">
         <v>1312</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I32" t="s">
         <v>7</v>
@@ -1511,22 +1511,22 @@
         <v>10</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D33" t="s">
         <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G33">
         <v>1312</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I33" t="s">
         <v>7</v>
@@ -1540,22 +1540,22 @@
         <v>10</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D34" t="s">
         <v>6</v>
       </c>
       <c r="E34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G34">
         <v>1312</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I34" t="s">
         <v>7</v>
@@ -1569,22 +1569,22 @@
         <v>10</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D35" t="s">
         <v>6</v>
       </c>
       <c r="E35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G35">
         <v>1312</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I35" t="s">
         <v>7</v>
@@ -1598,22 +1598,22 @@
         <v>10</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
       </c>
       <c r="E36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G36">
         <v>1312</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I36" t="s">
         <v>7</v>
@@ -1627,22 +1627,22 @@
         <v>10</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
       </c>
       <c r="E37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G37">
         <v>1312</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I37" t="s">
         <v>7</v>
@@ -1656,22 +1656,22 @@
         <v>10</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D38" t="s">
         <v>6</v>
       </c>
       <c r="E38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G38">
         <v>1312</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I38" t="s">
         <v>7</v>
@@ -1685,22 +1685,22 @@
         <v>10</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D39" t="s">
         <v>6</v>
       </c>
       <c r="E39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G39">
         <v>1312</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I39" t="s">
         <v>7</v>
@@ -1714,22 +1714,22 @@
         <v>10</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D40" t="s">
         <v>6</v>
       </c>
       <c r="E40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G40">
         <v>1312</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I40" t="s">
         <v>7</v>
@@ -1743,22 +1743,22 @@
         <v>10</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D41" t="s">
         <v>6</v>
       </c>
       <c r="E41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G41">
         <v>1312</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I41" t="s">
         <v>7</v>
@@ -1772,22 +1772,22 @@
         <v>10</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D42" t="s">
         <v>6</v>
       </c>
       <c r="E42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G42">
         <v>1312</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I42" t="s">
         <v>7</v>
@@ -1801,22 +1801,22 @@
         <v>10</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G43">
         <v>1312</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I43" t="s">
         <v>7</v>
@@ -1830,22 +1830,22 @@
         <v>10</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
       </c>
       <c r="E44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G44">
         <v>1312</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I44" t="s">
         <v>7</v>
@@ -1859,22 +1859,22 @@
         <v>10</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
       </c>
       <c r="E45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G45">
         <v>1312</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I45" t="s">
         <v>7</v>
@@ -1888,22 +1888,22 @@
         <v>10</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D46" t="s">
         <v>6</v>
       </c>
       <c r="E46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G46">
         <v>1312</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I46" t="s">
         <v>7</v>
@@ -1917,22 +1917,22 @@
         <v>10</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D47" t="s">
         <v>6</v>
       </c>
       <c r="E47" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G47">
         <v>1312</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I47" t="s">
         <v>7</v>
@@ -1946,22 +1946,22 @@
         <v>10</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D48" t="s">
         <v>6</v>
       </c>
       <c r="E48" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G48">
         <v>1312</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I48" t="s">
         <v>7</v>
@@ -1975,22 +1975,22 @@
         <v>10</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D49" t="s">
         <v>6</v>
       </c>
       <c r="E49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G49">
         <v>1312</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I49" t="s">
         <v>7</v>
@@ -2004,22 +2004,22 @@
         <v>10</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D50" t="s">
         <v>6</v>
       </c>
       <c r="E50" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G50">
         <v>1312</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I50" t="s">
         <v>7</v>
@@ -2033,22 +2033,22 @@
         <v>10</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D51" t="s">
         <v>6</v>
       </c>
       <c r="E51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G51">
         <v>1312</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I51" t="s">
         <v>7</v>
@@ -2062,22 +2062,22 @@
         <v>10</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D52" t="s">
         <v>6</v>
       </c>
       <c r="E52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G52">
         <v>1312</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I52" t="s">
         <v>7</v>
@@ -2091,22 +2091,22 @@
         <v>10</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D53" t="s">
         <v>6</v>
       </c>
       <c r="E53" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G53">
         <v>1312</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I53" t="s">
         <v>7</v>

</xml_diff>